<commit_message>
added data from August 2020 sequence run
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25306"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdstengl/Google_Drive/GitHub/viral_variant_explorer/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EA9458-B00B-C043-938D-9F618660F3EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="1460" windowWidth="36840" windowHeight="25160"/>
+    <workbookView xWindow="2360" yWindow="1460" windowWidth="36840" windowHeight="25160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata_v0" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata_v0!$A$1:$F$175</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="246">
   <si>
     <t>virus</t>
   </si>
@@ -685,12 +691,87 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>HIV_2_Group_F_1st_Generation_Mouse_1_W11</t>
+  </si>
+  <si>
+    <t>HIV</t>
+  </si>
+  <si>
+    <t>HIV_2_Group_F_1st_Generation_Mouse_1_W3</t>
+  </si>
+  <si>
+    <t>SIVB670_2nd_Generation_Mouse_J2873_W23</t>
+  </si>
+  <si>
+    <t>SIVB670_2nd_Generation_Mouse_J2878_W23</t>
+  </si>
+  <si>
+    <t>SIVB670_3rd_Generation_Mouse_B1076_W11</t>
+  </si>
+  <si>
+    <t>SIVB670_3rd_Generation_Mouse_B1076_W23</t>
+  </si>
+  <si>
+    <t>SIVB670_3rd_Generation_Mouse_B1076_W3</t>
+  </si>
+  <si>
+    <t>SIVB670_3rd_Generation_Mouse_B1077_W23</t>
+  </si>
+  <si>
+    <t>SIVB670_3rd_Generation_Mouse_B1077_W3</t>
+  </si>
+  <si>
+    <t>SIVcpzEK505_3rd_Generation_Mouse_2404_W3</t>
+  </si>
+  <si>
+    <t>J2404</t>
+  </si>
+  <si>
+    <t>SIVcpzLB715_3rd_Generation_Mouse_J12_W11</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>SIVcpzLB715_3rd_Generation_Mouse_J12_W19</t>
+  </si>
+  <si>
+    <t>SIVcpzLB715_3rd_Generation_Mouse_J12_W22</t>
+  </si>
+  <si>
+    <t>SIVcpzLB715_3rd_Generation_Mouse_J12_W3</t>
+  </si>
+  <si>
+    <t>SIVcpzLB715_3rd_Generation_Mouse_J4_W11</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>SIVcpzLB715_3rd_Generation_Mouse_J4_W19</t>
+  </si>
+  <si>
+    <t>SIVcpzLB715_3rd_Generation_Mouse_J4_W3</t>
+  </si>
+  <si>
+    <t>SIVcpzMB897_3rd_Generation_Mouse_J2904_W11</t>
+  </si>
+  <si>
+    <t>J2904</t>
+  </si>
+  <si>
+    <t>SIVcpzMB897_3rd_Generation_Mouse_J2904_W18</t>
+  </si>
+  <si>
+    <t>SIVcpzMB897_3rd_Generation_Mouse_J2904_W3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1557,28 +1638,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:F175"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F195"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176"/>
+    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>208</v>
       </c>
@@ -1598,7 +1678,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1618,7 +1698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1638,7 +1718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1658,7 +1738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1678,7 +1758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1698,7 +1778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1718,7 +1798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1738,7 +1818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1758,7 +1838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1778,7 +1858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1798,7 +1878,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1818,7 +1898,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1838,7 +1918,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1858,7 +1938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1878,7 +1958,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1898,7 +1978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1918,7 +1998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1938,7 +2018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1958,7 +2038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1978,7 +2058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1998,7 +2078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -2018,7 +2098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -2038,7 +2118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -2058,7 +2138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -2078,7 +2158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -2098,7 +2178,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -2118,7 +2198,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -2138,7 +2218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -2158,7 +2238,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -2178,7 +2258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -2198,7 +2278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -2218,7 +2298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -2238,7 +2318,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -2258,7 +2338,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -2278,7 +2358,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -2298,7 +2378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -2318,7 +2398,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -2338,7 +2418,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -2358,7 +2438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -2378,7 +2458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -2398,7 +2478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2418,7 +2498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -2438,7 +2518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -2458,7 +2538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -2478,7 +2558,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -2498,7 +2578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -2518,7 +2598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -2538,7 +2618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -2558,7 +2638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -2578,7 +2658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -2598,7 +2678,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>69</v>
       </c>
@@ -2618,7 +2698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -2638,7 +2718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -2658,7 +2738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>73</v>
       </c>
@@ -2678,7 +2758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>74</v>
       </c>
@@ -2698,7 +2778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>75</v>
       </c>
@@ -2718,7 +2798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>76</v>
       </c>
@@ -2738,7 +2818,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>77</v>
       </c>
@@ -2758,7 +2838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -2778,7 +2858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>79</v>
       </c>
@@ -2798,7 +2878,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>80</v>
       </c>
@@ -2818,7 +2898,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>81</v>
       </c>
@@ -2838,7 +2918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -2858,7 +2938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>83</v>
       </c>
@@ -2878,7 +2958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>84</v>
       </c>
@@ -2898,7 +2978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>85</v>
       </c>
@@ -2918,7 +2998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>86</v>
       </c>
@@ -2938,7 +3018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>87</v>
       </c>
@@ -2958,7 +3038,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>88</v>
       </c>
@@ -2978,7 +3058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>89</v>
       </c>
@@ -2998,7 +3078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>90</v>
       </c>
@@ -3018,7 +3098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>119</v>
       </c>
@@ -3038,7 +3118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>101</v>
       </c>
@@ -3058,7 +3138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>103</v>
       </c>
@@ -3078,7 +3158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>104</v>
       </c>
@@ -3098,7 +3178,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>105</v>
       </c>
@@ -3118,7 +3198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>106</v>
       </c>
@@ -3138,7 +3218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>108</v>
       </c>
@@ -3158,7 +3238,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>109</v>
       </c>
@@ -3178,7 +3258,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>110</v>
       </c>
@@ -3198,7 +3278,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>91</v>
       </c>
@@ -3218,7 +3298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>94</v>
       </c>
@@ -3238,7 +3318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>95</v>
       </c>
@@ -3258,7 +3338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>96</v>
       </c>
@@ -3278,7 +3358,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>98</v>
       </c>
@@ -3298,7 +3378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>99</v>
       </c>
@@ -3318,7 +3398,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>100</v>
       </c>
@@ -3338,7 +3418,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>111</v>
       </c>
@@ -3358,7 +3438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>113</v>
       </c>
@@ -3378,7 +3458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>114</v>
       </c>
@@ -3398,7 +3478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>115</v>
       </c>
@@ -3418,7 +3498,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>117</v>
       </c>
@@ -3438,7 +3518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>118</v>
       </c>
@@ -3458,7 +3538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>153</v>
       </c>
@@ -3478,7 +3558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>120</v>
       </c>
@@ -3498,7 +3578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>123</v>
       </c>
@@ -3518,7 +3598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>124</v>
       </c>
@@ -3538,7 +3618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>125</v>
       </c>
@@ -3558,7 +3638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>127</v>
       </c>
@@ -3578,7 +3658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>128</v>
       </c>
@@ -3598,7 +3678,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>129</v>
       </c>
@@ -3618,7 +3698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>130</v>
       </c>
@@ -3638,7 +3718,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>212</v>
       </c>
@@ -3658,7 +3738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>131</v>
       </c>
@@ -3678,7 +3758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>133</v>
       </c>
@@ -3698,7 +3778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>135</v>
       </c>
@@ -3718,7 +3798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>136</v>
       </c>
@@ -3738,7 +3818,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>137</v>
       </c>
@@ -3758,7 +3838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>138</v>
       </c>
@@ -3778,7 +3858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>139</v>
       </c>
@@ -3798,7 +3878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>213</v>
       </c>
@@ -3818,7 +3898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>214</v>
       </c>
@@ -3838,7 +3918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>215</v>
       </c>
@@ -3858,7 +3938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>216</v>
       </c>
@@ -3878,7 +3958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>217</v>
       </c>
@@ -3898,7 +3978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>145</v>
       </c>
@@ -3918,7 +3998,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>147</v>
       </c>
@@ -3938,7 +4018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>148</v>
       </c>
@@ -3958,7 +4038,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>140</v>
       </c>
@@ -3978,7 +4058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>142</v>
       </c>
@@ -3998,7 +4078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>143</v>
       </c>
@@ -4018,7 +4098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>144</v>
       </c>
@@ -4038,7 +4118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>149</v>
       </c>
@@ -4058,7 +4138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>151</v>
       </c>
@@ -4078,7 +4158,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>152</v>
       </c>
@@ -4098,7 +4178,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>207</v>
       </c>
@@ -4118,7 +4198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>177</v>
       </c>
@@ -4138,7 +4218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>178</v>
       </c>
@@ -4158,7 +4238,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>179</v>
       </c>
@@ -4178,7 +4258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>180</v>
       </c>
@@ -4198,7 +4278,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>181</v>
       </c>
@@ -4218,7 +4298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>182</v>
       </c>
@@ -4238,7 +4318,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>183</v>
       </c>
@@ -4258,7 +4338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>184</v>
       </c>
@@ -4278,7 +4358,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>185</v>
       </c>
@@ -4298,7 +4378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>186</v>
       </c>
@@ -4318,7 +4398,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>187</v>
       </c>
@@ -4338,7 +4418,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>188</v>
       </c>
@@ -4358,7 +4438,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="140" spans="1:6" hidden="1">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>189</v>
       </c>
@@ -4378,7 +4458,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="141" spans="1:6" hidden="1">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>191</v>
       </c>
@@ -4398,7 +4478,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>192</v>
       </c>
@@ -4418,7 +4498,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>154</v>
       </c>
@@ -4438,7 +4518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>194</v>
       </c>
@@ -4458,7 +4538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>195</v>
       </c>
@@ -4478,7 +4558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:6" hidden="1">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>196</v>
       </c>
@@ -4498,7 +4578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:6" hidden="1">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>197</v>
       </c>
@@ -4518,7 +4598,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>199</v>
       </c>
@@ -4538,7 +4618,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>200</v>
       </c>
@@ -4558,7 +4638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>157</v>
       </c>
@@ -4578,7 +4658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>158</v>
       </c>
@@ -4598,7 +4678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>159</v>
       </c>
@@ -4618,7 +4698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>160</v>
       </c>
@@ -4638,7 +4718,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>161</v>
       </c>
@@ -4658,7 +4738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="1:6" hidden="1">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>162</v>
       </c>
@@ -4678,7 +4758,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:6" hidden="1">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>163</v>
       </c>
@@ -4698,7 +4778,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="157" spans="1:6" hidden="1">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>164</v>
       </c>
@@ -4718,7 +4798,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>201</v>
       </c>
@@ -4738,7 +4818,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>202</v>
       </c>
@@ -4758,7 +4838,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="160" spans="1:6" hidden="1">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>203</v>
       </c>
@@ -4778,7 +4858,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>204</v>
       </c>
@@ -4798,7 +4878,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="162" spans="1:6" hidden="1">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>205</v>
       </c>
@@ -4818,7 +4898,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>206</v>
       </c>
@@ -4838,7 +4918,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>165</v>
       </c>
@@ -4858,7 +4938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>166</v>
       </c>
@@ -4878,7 +4958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>167</v>
       </c>
@@ -4898,7 +4978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>168</v>
       </c>
@@ -4918,7 +4998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:6" hidden="1">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>169</v>
       </c>
@@ -4938,7 +5018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>170</v>
       </c>
@@ -4958,7 +5038,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>171</v>
       </c>
@@ -4978,7 +5058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>172</v>
       </c>
@@ -4998,7 +5078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:6" hidden="1">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>173</v>
       </c>
@@ -5018,7 +5098,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="173" spans="1:6" hidden="1">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>174</v>
       </c>
@@ -5038,7 +5118,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="174" spans="1:6" hidden="1">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>175</v>
       </c>
@@ -5058,7 +5138,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>176</v>
       </c>
@@ -5078,14 +5158,409 @@
         <v>219</v>
       </c>
     </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>221</v>
+      </c>
+      <c r="B176" t="s">
+        <v>222</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+      <c r="D176">
+        <v>11</v>
+      </c>
+      <c r="E176">
+        <v>1</v>
+      </c>
+      <c r="F176" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>223</v>
+      </c>
+      <c r="B177" t="s">
+        <v>222</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+      <c r="D177">
+        <v>3</v>
+      </c>
+      <c r="E177">
+        <v>1</v>
+      </c>
+      <c r="F177" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>224</v>
+      </c>
+      <c r="B178" t="s">
+        <v>3</v>
+      </c>
+      <c r="C178">
+        <v>2</v>
+      </c>
+      <c r="D178">
+        <v>23</v>
+      </c>
+      <c r="E178" t="s">
+        <v>22</v>
+      </c>
+      <c r="F178" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>225</v>
+      </c>
+      <c r="B179" t="s">
+        <v>3</v>
+      </c>
+      <c r="C179">
+        <v>2</v>
+      </c>
+      <c r="D179">
+        <v>23</v>
+      </c>
+      <c r="E179" t="s">
+        <v>4</v>
+      </c>
+      <c r="F179" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>226</v>
+      </c>
+      <c r="B180" t="s">
+        <v>3</v>
+      </c>
+      <c r="C180">
+        <v>3</v>
+      </c>
+      <c r="D180">
+        <v>11</v>
+      </c>
+      <c r="E180" t="s">
+        <v>9</v>
+      </c>
+      <c r="F180" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>227</v>
+      </c>
+      <c r="B181" t="s">
+        <v>3</v>
+      </c>
+      <c r="C181">
+        <v>3</v>
+      </c>
+      <c r="D181">
+        <v>23</v>
+      </c>
+      <c r="E181" t="s">
+        <v>9</v>
+      </c>
+      <c r="F181" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>228</v>
+      </c>
+      <c r="B182" t="s">
+        <v>3</v>
+      </c>
+      <c r="C182">
+        <v>3</v>
+      </c>
+      <c r="D182">
+        <v>3</v>
+      </c>
+      <c r="E182" t="s">
+        <v>9</v>
+      </c>
+      <c r="F182" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>229</v>
+      </c>
+      <c r="B183" t="s">
+        <v>3</v>
+      </c>
+      <c r="C183">
+        <v>3</v>
+      </c>
+      <c r="D183">
+        <v>23</v>
+      </c>
+      <c r="E183" t="s">
+        <v>11</v>
+      </c>
+      <c r="F183" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>230</v>
+      </c>
+      <c r="B184" t="s">
+        <v>3</v>
+      </c>
+      <c r="C184">
+        <v>3</v>
+      </c>
+      <c r="D184">
+        <v>3</v>
+      </c>
+      <c r="E184" t="s">
+        <v>11</v>
+      </c>
+      <c r="F184" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>231</v>
+      </c>
+      <c r="B185" t="s">
+        <v>28</v>
+      </c>
+      <c r="C185">
+        <v>3</v>
+      </c>
+      <c r="D185">
+        <v>3</v>
+      </c>
+      <c r="E185" t="s">
+        <v>232</v>
+      </c>
+      <c r="F185" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>233</v>
+      </c>
+      <c r="B186" t="s">
+        <v>51</v>
+      </c>
+      <c r="C186">
+        <v>3</v>
+      </c>
+      <c r="D186">
+        <v>11</v>
+      </c>
+      <c r="E186" t="s">
+        <v>234</v>
+      </c>
+      <c r="F186" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>235</v>
+      </c>
+      <c r="B187" t="s">
+        <v>51</v>
+      </c>
+      <c r="C187">
+        <v>3</v>
+      </c>
+      <c r="D187">
+        <v>19</v>
+      </c>
+      <c r="E187" t="s">
+        <v>234</v>
+      </c>
+      <c r="F187" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>236</v>
+      </c>
+      <c r="B188" t="s">
+        <v>51</v>
+      </c>
+      <c r="C188">
+        <v>3</v>
+      </c>
+      <c r="D188">
+        <v>22</v>
+      </c>
+      <c r="E188" t="s">
+        <v>234</v>
+      </c>
+      <c r="F188" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>237</v>
+      </c>
+      <c r="B189" t="s">
+        <v>51</v>
+      </c>
+      <c r="C189">
+        <v>3</v>
+      </c>
+      <c r="D189">
+        <v>3</v>
+      </c>
+      <c r="E189" t="s">
+        <v>234</v>
+      </c>
+      <c r="F189" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>238</v>
+      </c>
+      <c r="B190" t="s">
+        <v>51</v>
+      </c>
+      <c r="C190">
+        <v>3</v>
+      </c>
+      <c r="D190">
+        <v>11</v>
+      </c>
+      <c r="E190" t="s">
+        <v>239</v>
+      </c>
+      <c r="F190" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>240</v>
+      </c>
+      <c r="B191" t="s">
+        <v>51</v>
+      </c>
+      <c r="C191">
+        <v>3</v>
+      </c>
+      <c r="D191">
+        <v>19</v>
+      </c>
+      <c r="E191" t="s">
+        <v>239</v>
+      </c>
+      <c r="F191" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>241</v>
+      </c>
+      <c r="B192" t="s">
+        <v>51</v>
+      </c>
+      <c r="C192">
+        <v>3</v>
+      </c>
+      <c r="D192">
+        <v>3</v>
+      </c>
+      <c r="E192" t="s">
+        <v>239</v>
+      </c>
+      <c r="F192" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>242</v>
+      </c>
+      <c r="B193" t="s">
+        <v>72</v>
+      </c>
+      <c r="C193">
+        <v>3</v>
+      </c>
+      <c r="D193">
+        <v>11</v>
+      </c>
+      <c r="E193" t="s">
+        <v>243</v>
+      </c>
+      <c r="F193" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>244</v>
+      </c>
+      <c r="B194" t="s">
+        <v>72</v>
+      </c>
+      <c r="C194">
+        <v>3</v>
+      </c>
+      <c r="D194">
+        <v>18</v>
+      </c>
+      <c r="E194" t="s">
+        <v>243</v>
+      </c>
+      <c r="F194" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>245</v>
+      </c>
+      <c r="B195" t="s">
+        <v>72</v>
+      </c>
+      <c r="C195">
+        <v>3</v>
+      </c>
+      <c r="D195">
+        <v>3</v>
+      </c>
+      <c r="E195" t="s">
+        <v>243</v>
+      </c>
+      <c r="F195" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F175">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="SIVhu"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A73:F94">
+  <autoFilter ref="A1:F175" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A73:F94">
       <sortCondition ref="C1:C175"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
August 2020 sequence data updates
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdstengl/Google_Drive/GitHub/viral_variant_explorer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EA9458-B00B-C043-938D-9F618660F3EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8D2DAE-3C1E-C443-9175-B5E37734CF5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="1460" windowWidth="36840" windowHeight="25160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2360" yWindow="1420" windowWidth="36840" windowHeight="25160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata_v0" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata_v0!$A$1:$F$175</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata_v0!$A$1:$F$195</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
   <extLst>
@@ -1392,7 +1392,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1444,7 +1444,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1646,10 +1646,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A176" sqref="A176"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="C199" sqref="C199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1738,7 +1739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1758,7 +1759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1778,7 +1779,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1818,7 +1819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1838,7 +1839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1858,7 +1859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1878,7 +1879,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1898,7 +1899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1918,7 +1919,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1995,10 +1996,10 @@
         <v>22</v>
       </c>
       <c r="F17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2018,7 +2019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2038,7 +2039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -2058,7 +2059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -2078,7 +2079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -2098,7 +2099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -2118,7 +2119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -2138,7 +2139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -2158,7 +2159,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -2178,7 +2179,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -2198,7 +2199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -2218,7 +2219,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -2238,7 +2239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -2258,7 +2259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -2278,7 +2279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -2298,7 +2299,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -2318,7 +2319,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -2338,7 +2339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -2358,7 +2359,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -2378,7 +2379,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -2398,7 +2399,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -2418,7 +2419,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -2438,7 +2439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -2458,7 +2459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -2478,7 +2479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2498,7 +2499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -2538,7 +2539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -2558,7 +2559,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -2578,7 +2579,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -2598,7 +2599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -2618,7 +2619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -2638,7 +2639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -2658,7 +2659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -2678,7 +2679,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>69</v>
       </c>
@@ -2698,7 +2699,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -2718,7 +2719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>71</v>
       </c>
@@ -2738,7 +2739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>73</v>
       </c>
@@ -2758,7 +2759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>74</v>
       </c>
@@ -2778,7 +2779,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>75</v>
       </c>
@@ -2798,7 +2799,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>76</v>
       </c>
@@ -2818,7 +2819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>77</v>
       </c>
@@ -2838,7 +2839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -2858,7 +2859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>79</v>
       </c>
@@ -2878,7 +2879,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>80</v>
       </c>
@@ -2898,7 +2899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>81</v>
       </c>
@@ -2918,7 +2919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -2938,7 +2939,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>83</v>
       </c>
@@ -2958,7 +2959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>84</v>
       </c>
@@ -2978,7 +2979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>85</v>
       </c>
@@ -2998,7 +2999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>86</v>
       </c>
@@ -3018,7 +3019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>87</v>
       </c>
@@ -3038,7 +3039,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>88</v>
       </c>
@@ -3058,7 +3059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>89</v>
       </c>
@@ -3078,7 +3079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>90</v>
       </c>
@@ -3098,7 +3099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>119</v>
       </c>
@@ -3118,7 +3119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>101</v>
       </c>
@@ -3138,7 +3139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>103</v>
       </c>
@@ -3158,7 +3159,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>104</v>
       </c>
@@ -3178,7 +3179,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>105</v>
       </c>
@@ -3198,7 +3199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>106</v>
       </c>
@@ -3218,7 +3219,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>108</v>
       </c>
@@ -3238,7 +3239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>109</v>
       </c>
@@ -3258,7 +3259,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>110</v>
       </c>
@@ -3278,7 +3279,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>91</v>
       </c>
@@ -3298,7 +3299,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>94</v>
       </c>
@@ -3318,7 +3319,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>95</v>
       </c>
@@ -3338,7 +3339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>96</v>
       </c>
@@ -3358,7 +3359,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>98</v>
       </c>
@@ -3378,7 +3379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>99</v>
       </c>
@@ -3398,7 +3399,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>100</v>
       </c>
@@ -3418,7 +3419,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>111</v>
       </c>
@@ -3438,7 +3439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>113</v>
       </c>
@@ -3458,7 +3459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>114</v>
       </c>
@@ -3478,7 +3479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>115</v>
       </c>
@@ -3498,7 +3499,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>117</v>
       </c>
@@ -3518,7 +3519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>118</v>
       </c>
@@ -3538,7 +3539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>153</v>
       </c>
@@ -3558,7 +3559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>120</v>
       </c>
@@ -3578,7 +3579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>123</v>
       </c>
@@ -3598,7 +3599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>124</v>
       </c>
@@ -3618,7 +3619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>125</v>
       </c>
@@ -3638,7 +3639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>127</v>
       </c>
@@ -3658,7 +3659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>128</v>
       </c>
@@ -3678,7 +3679,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>129</v>
       </c>
@@ -3698,7 +3699,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>130</v>
       </c>
@@ -3718,7 +3719,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>212</v>
       </c>
@@ -3738,7 +3739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>131</v>
       </c>
@@ -3758,7 +3759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>133</v>
       </c>
@@ -3778,7 +3779,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>135</v>
       </c>
@@ -3798,7 +3799,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>136</v>
       </c>
@@ -3818,7 +3819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>137</v>
       </c>
@@ -3838,7 +3839,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>138</v>
       </c>
@@ -3858,7 +3859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>139</v>
       </c>
@@ -3878,7 +3879,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>213</v>
       </c>
@@ -3898,7 +3899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>214</v>
       </c>
@@ -3918,7 +3919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>215</v>
       </c>
@@ -3938,7 +3939,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>216</v>
       </c>
@@ -3958,7 +3959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>217</v>
       </c>
@@ -3978,7 +3979,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>145</v>
       </c>
@@ -3998,7 +3999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>147</v>
       </c>
@@ -4018,7 +4019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>148</v>
       </c>
@@ -4038,7 +4039,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>140</v>
       </c>
@@ -4058,7 +4059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>142</v>
       </c>
@@ -4078,7 +4079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>143</v>
       </c>
@@ -4098,7 +4099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>144</v>
       </c>
@@ -4118,7 +4119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>149</v>
       </c>
@@ -4138,7 +4139,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>151</v>
       </c>
@@ -4158,7 +4159,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>152</v>
       </c>
@@ -4178,7 +4179,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>207</v>
       </c>
@@ -4198,7 +4199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>177</v>
       </c>
@@ -4218,7 +4219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>178</v>
       </c>
@@ -4238,7 +4239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>179</v>
       </c>
@@ -4258,7 +4259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>180</v>
       </c>
@@ -4278,7 +4279,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>181</v>
       </c>
@@ -4298,7 +4299,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>182</v>
       </c>
@@ -4318,7 +4319,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>183</v>
       </c>
@@ -4338,7 +4339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>184</v>
       </c>
@@ -4358,7 +4359,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>185</v>
       </c>
@@ -4378,7 +4379,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>186</v>
       </c>
@@ -4398,7 +4399,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>187</v>
       </c>
@@ -4418,7 +4419,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>188</v>
       </c>
@@ -4438,7 +4439,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>189</v>
       </c>
@@ -4458,7 +4459,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>191</v>
       </c>
@@ -4478,7 +4479,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>192</v>
       </c>
@@ -4498,7 +4499,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>154</v>
       </c>
@@ -4518,7 +4519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>194</v>
       </c>
@@ -4538,7 +4539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>195</v>
       </c>
@@ -4558,7 +4559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>196</v>
       </c>
@@ -4578,7 +4579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>197</v>
       </c>
@@ -4598,7 +4599,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>199</v>
       </c>
@@ -4618,7 +4619,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>200</v>
       </c>
@@ -4638,7 +4639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>157</v>
       </c>
@@ -4658,7 +4659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>158</v>
       </c>
@@ -4678,7 +4679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>159</v>
       </c>
@@ -4698,7 +4699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>160</v>
       </c>
@@ -4718,7 +4719,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>161</v>
       </c>
@@ -4738,7 +4739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>162</v>
       </c>
@@ -4758,7 +4759,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>163</v>
       </c>
@@ -4778,7 +4779,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>164</v>
       </c>
@@ -4798,7 +4799,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>201</v>
       </c>
@@ -4818,7 +4819,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>202</v>
       </c>
@@ -4838,7 +4839,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>203</v>
       </c>
@@ -4858,7 +4859,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>204</v>
       </c>
@@ -4878,7 +4879,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>205</v>
       </c>
@@ -4898,7 +4899,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>206</v>
       </c>
@@ -4918,7 +4919,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>165</v>
       </c>
@@ -4938,7 +4939,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>166</v>
       </c>
@@ -4958,7 +4959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>167</v>
       </c>
@@ -4978,7 +4979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>168</v>
       </c>
@@ -4998,7 +4999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>169</v>
       </c>
@@ -5018,7 +5019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>170</v>
       </c>
@@ -5038,7 +5039,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>171</v>
       </c>
@@ -5058,7 +5059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>172</v>
       </c>
@@ -5078,7 +5079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>173</v>
       </c>
@@ -5098,7 +5099,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>174</v>
       </c>
@@ -5118,7 +5119,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>175</v>
       </c>
@@ -5138,7 +5139,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>176</v>
       </c>
@@ -5158,7 +5159,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>221</v>
       </c>
@@ -5178,7 +5179,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>223</v>
       </c>
@@ -5215,7 +5216,7 @@
         <v>22</v>
       </c>
       <c r="F178" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -5235,10 +5236,10 @@
         <v>4</v>
       </c>
       <c r="F179" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>226</v>
       </c>
@@ -5258,7 +5259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>227</v>
       </c>
@@ -5278,7 +5279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>228</v>
       </c>
@@ -5298,7 +5299,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>229</v>
       </c>
@@ -5318,7 +5319,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>230</v>
       </c>
@@ -5338,7 +5339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>231</v>
       </c>
@@ -5358,7 +5359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>233</v>
       </c>
@@ -5378,7 +5379,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>235</v>
       </c>
@@ -5398,7 +5399,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>236</v>
       </c>
@@ -5418,7 +5419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>237</v>
       </c>
@@ -5438,7 +5439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>238</v>
       </c>
@@ -5458,7 +5459,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>240</v>
       </c>
@@ -5478,7 +5479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>241</v>
       </c>
@@ -5498,7 +5499,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>242</v>
       </c>
@@ -5518,7 +5519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>244</v>
       </c>
@@ -5538,7 +5539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>245</v>
       </c>
@@ -5559,7 +5560,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F175" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:F195" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="SIVB670"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A73:F94">
       <sortCondition ref="C1:C175"/>
     </sortState>

</xml_diff>